<commit_message>
updated mock data files
</commit_message>
<xml_diff>
--- a/Excel/MockData/Negative Comments - August 19.xlsx
+++ b/Excel/MockData/Negative Comments - August 19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chak\Documents\Other\Mock Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B24443E-603D-490C-A246-EBAF1B662425}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB896EE-A205-40C1-85F3-9956A6AE531C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27975" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>CLINIC</t>
   </si>
@@ -31,64 +31,64 @@
     <t>COMMENTS</t>
   </si>
   <si>
+    <t>Extremely Unlikely</t>
+  </si>
+  <si>
+    <t>Waited too long to find a parking spot</t>
+  </si>
+  <si>
+    <t>Radiology</t>
+  </si>
+  <si>
+    <t>Doctors are patronising and made me feel bad</t>
+  </si>
+  <si>
+    <t>Orthodontics</t>
+  </si>
+  <si>
+    <t>Special Care Baby Unit</t>
+  </si>
+  <si>
+    <t>Long wait times</t>
+  </si>
+  <si>
+    <t>Unlikely</t>
+  </si>
+  <si>
+    <t>Heart Failure</t>
+  </si>
+  <si>
+    <t>Day Surgery</t>
+  </si>
+  <si>
+    <t>Waited over 5 hours</t>
+  </si>
+  <si>
+    <t>Food was terrible</t>
+  </si>
+  <si>
+    <t>Clenliness isn't the best but otherwise okay</t>
+  </si>
+  <si>
+    <t>staff tried to deal with me quickly rather than correctly. Not appropriate and i shouldve have been taken care of better. Would not recommend.</t>
+  </si>
+  <si>
+    <t>Rehab Services</t>
+  </si>
+  <si>
+    <t>I waited for a long time to be turned away</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
     <t>Bone Health</t>
   </si>
   <si>
-    <t>Extremely Unlikely</t>
-  </si>
-  <si>
-    <t>doctors dont seem to care</t>
-  </si>
-  <si>
-    <t>Radiology</t>
-  </si>
-  <si>
-    <t>Unlikely</t>
-  </si>
-  <si>
-    <t>Doctors are patronising</t>
-  </si>
-  <si>
-    <t>Theatre Treatment Suite Implants</t>
-  </si>
-  <si>
-    <t>staff tried to deal with me quickly rather than correctly</t>
-  </si>
-  <si>
     <t>Gynaecology</t>
   </si>
   <si>
-    <t>Service recieved was adaquete but staff seemed to not care</t>
-  </si>
-  <si>
-    <t>Dermatology</t>
-  </si>
-  <si>
-    <t>staff was rude</t>
-  </si>
-  <si>
-    <t>A&amp;E</t>
-  </si>
-  <si>
-    <t>Clenliness isn't the best but otherwise okay</t>
-  </si>
-  <si>
-    <t>Special Care Baby Unit</t>
-  </si>
-  <si>
-    <t>Food was terrible</t>
-  </si>
-  <si>
-    <t>Day Surgery</t>
-  </si>
-  <si>
-    <t>Waited too long to find a parking spot</t>
-  </si>
-  <si>
     <t>Waited for long time for poor service</t>
-  </si>
-  <si>
-    <t>Long wait times</t>
   </si>
 </sst>
 </file>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A82" sqref="A17:XFD82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,109 +459,109 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -569,79 +569,57 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>